<commit_message>
Update CEA results: modify and replace `rsv_cea_results.xlsx`
</commit_message>
<xml_diff>
--- a/rsv_cea_results.xlsx
+++ b/rsv_cea_results.xlsx
@@ -1,21 +1,98 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fandtlabs-my.sharepoint.com/personal/jefferson_fandtlabs_com/Documents/Academic/Course Content/Economic Evaluation 3/rsv-vaccination-envaluation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_EC68FDCE8F79A8D366075C52F3D99A770587C71A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA445E8C-36FD-8B46-9164-00C01F907B2C}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="600" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Total_Periods</t>
+  </si>
+  <si>
+    <t>Total Cost (Millions)</t>
+  </si>
+  <si>
+    <t>Total QALY (Millions)</t>
+  </si>
+  <si>
+    <t>Incremental Cost (Millions)</t>
+  </si>
+  <si>
+    <t>Incremental QALY (Millions)</t>
+  </si>
+  <si>
+    <t>ICER ($/QALY)</t>
+  </si>
+  <si>
+    <t>Standard of Care</t>
+  </si>
+  <si>
+    <t>$717,536.37</t>
+  </si>
+  <si>
+    <t>660.44</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Abrysvo</t>
+  </si>
+  <si>
+    <t>$683,436.19</t>
+  </si>
+  <si>
+    <t>660.63</t>
+  </si>
+  <si>
+    <t>$-34,100.18</t>
+  </si>
+  <si>
+    <t>0.19</t>
+  </si>
+  <si>
+    <t>$-183,055.28</t>
+  </si>
+  <si>
+    <t>Arexvy</t>
+  </si>
+  <si>
+    <t>$680,396.58</t>
+  </si>
+  <si>
+    <t>$-3,039.61</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>$-1,318,307.95</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +140,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -107,7 +192,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -141,6 +226,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -175,9 +261,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -350,153 +437,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Scenario</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Total_Periods</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Total Cost (Millions)</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Total QALY (Millions)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Incremental Cost (Millions)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Incremental QALY (Millions)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ICER ($/QALY)</t>
-        </is>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Standard of Care</t>
-        </is>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2">
         <v>12878</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>$717,536.37</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>660.44</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Abrysvo</t>
-        </is>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3">
         <v>12500</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>$683,436.19</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>660.63</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>$-34,100.18</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>0.19</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>$-183,055.28</t>
-        </is>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Arexvy</t>
-        </is>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
       </c>
       <c r="B4">
         <v>12500</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>$680,396.58</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>660.63</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>$-3,039.61</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>0.00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>$-1,318,307.95</t>
-        </is>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>